<commit_message>
- Search Functionality - Minor UI Tweaks - 15 titles added
</commit_message>
<xml_diff>
--- a/WordCloudCreator/wwwroot/List of Titles/Title List.xlsx
+++ b/WordCloudCreator/wwwroot/List of Titles/Title List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billz\source\repos\WordCloudCreator\WordCloudCreator\wwwroot\List of Titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75647AA3-5A1E-4217-BA61-908E2824376A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF08ABB-177F-488E-938D-2ECE2A7F28CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" activeTab="1" xr2:uid="{0C4333F4-DFAB-4B7F-B221-4737101A17F3}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" activeTab="3" xr2:uid="{0C4333F4-DFAB-4B7F-B221-4737101A17F3}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
   <si>
     <t>Action</t>
   </si>
@@ -211,9 +211,6 @@
 </t>
   </si>
   <si>
-    <t>MediaTitle7</t>
-  </si>
-  <si>
     <t>Political pressure mounts to install a system of accountability when the actions of the Avengers lead to collateral damage. The new status quo deeply divides members of the team.</t>
   </si>
   <si>
@@ -266,6 +263,103 @@
   </si>
   <si>
     <t>Genre: Crime, Drama, Biography, Thriller</t>
+  </si>
+  <si>
+    <t>Die Hard</t>
+  </si>
+  <si>
+    <t>mediaTitle_0011</t>
+  </si>
+  <si>
+    <t>mediaTitle_0007</t>
+  </si>
+  <si>
+    <t>mediaTitle_0012</t>
+  </si>
+  <si>
+    <t>mediaTitle_0013</t>
+  </si>
+  <si>
+    <t>mediaTitle_0014</t>
+  </si>
+  <si>
+    <t>mediaTitle_0015</t>
+  </si>
+  <si>
+    <t>District 9</t>
+  </si>
+  <si>
+    <t>Spider-Man: Far From Home</t>
+  </si>
+  <si>
+    <t>I, Robot</t>
+  </si>
+  <si>
+    <t>Face/Off</t>
+  </si>
+  <si>
+    <t>Die Hard | 1988 | 2h 12m</t>
+  </si>
+  <si>
+    <t>Genre: Action, Thriller</t>
+  </si>
+  <si>
+    <t>District 9 | 2009 | 1h 52m</t>
+  </si>
+  <si>
+    <t>Violence ensues after an extraterrestrial race forced to live in slum-like conditions on Earth finds a kindred spirit in a government agent exposed to their biotechnology.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A New York City police officer tries to save his estranged wife and several others taken hostage by terrorists during a Christmas party at the Nakatomi Plaza in Los Angeles.
+</t>
+  </si>
+  <si>
+    <t>Cast: Sharlto Copley, Jason Cope, David James, Vanessa Haywood, Mandla Gaduka, Kenneth Nkosi, Eugene Khumbanyiwa, Louis Minnaar, William Allen Young</t>
+  </si>
+  <si>
+    <t>Cast: Bruce Willis, Alan Rickman, Alexander Godunov, Bonnie Bedelia</t>
+  </si>
+  <si>
+    <t>Genre: Action, Adventure, Sci-Fi, Fantasy, Horror</t>
+  </si>
+  <si>
+    <t>Spider-Man: Far From Home | 2019 | 2h 10m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Following the events of Avengers: Endgame (2019), Spider-Man must step up to take on new threats in a world that has changed forever.
+</t>
+  </si>
+  <si>
+    <t>Cast: Tom Holland, Samuel L. Jackson, Zendaya, Cobie Smulders, Jon Favreau, J. B. Smoove, Jacob Batalon, Martin Starr, Tony Revolori, Marisa Tomei, Jake Gyllenhaal</t>
+  </si>
+  <si>
+    <t>Genre: Action, Superhero, Sci-Fi, Comedy</t>
+  </si>
+  <si>
+    <t>I, Robot | 2004 | 1h 55m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2035, a technophobic cop investigates a crime that may have been perpetrated by a robot, which leads to a larger threat to humanity.
+</t>
+  </si>
+  <si>
+    <t>Cast: Will Smith, Bridget Moynahan, Bruce Greenwood, James Cromwell, Chi McBride, Alan Tudyk</t>
+  </si>
+  <si>
+    <t>Genre: Sci-Fi, Action, Crime, Mystery, Thriller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To foil a terrorist plot, an FBI agent undergoes facial transplant surgery to assume the identity of the criminal mastermind who murdered his only son, but the criminal wakes up prematurely and seeks revenge.
+</t>
+  </si>
+  <si>
+    <t>Face/Off | 1997 | 2h 13m</t>
+  </si>
+  <si>
+    <t>Cast: John Travolta, Nicolas Cage, Joan Allen, Gina Gershon, Alessandro Nivola, Colm Feore</t>
+  </si>
+  <si>
+    <t>Genre: Action, Crime, Sci-Fi, Thriller</t>
   </si>
 </sst>
 </file>
@@ -737,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223C6D44-3CDC-4FE4-8810-0D37E5E3FC32}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
@@ -777,19 +871,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -877,39 +971,39 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -950,9 +1044,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625AA347-218C-4A8D-8B5F-45528BD680D9}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -985,62 +1079,128 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="90.35" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="3" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- New Collection Pages - "Similar Titles" for each title - Row Scroll Button Functionality - Mobile Viewport
</commit_message>
<xml_diff>
--- a/WordCloudCreator/wwwroot/List of Titles/Title List.xlsx
+++ b/WordCloudCreator/wwwroot/List of Titles/Title List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billz\source\repos\WordCloudCreator\WordCloudCreator\wwwroot\List of Titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF08ABB-177F-488E-938D-2ECE2A7F28CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A8E138-339D-4B09-B0D7-0A1E032A8F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" activeTab="3" xr2:uid="{0C4333F4-DFAB-4B7F-B221-4737101A17F3}"/>
   </bookViews>
@@ -833,7 +833,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -933,7 +933,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1046,7 +1046,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1212,7 +1212,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="A1:F2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>